<commit_message>
Payment worker first part inspection
</commit_message>
<xml_diff>
--- a/5_CodeInspection/Code_checks_Erica_v1.xlsx
+++ b/5_CodeInspection/Code_checks_Erica_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BillingAccountWorker" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="118">
   <si>
     <t>2.1 Naming Conventions</t>
   </si>
@@ -346,6 +346,39 @@
   </si>
   <si>
     <t>OK ?</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>nd</t>
+  </si>
+  <si>
+    <t>module, decimals and rounding should be uppercase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getPaymentMethodAndRelated: lines 103, 107, </t>
+  </si>
+  <si>
+    <t>ok blanks, comments are missing</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>no: 99,128-132,519,165, getPaymentApplied:288,193-308</t>
+  </si>
+  <si>
+    <t>getPaymentMethodAndRelated java doc missing</t>
+  </si>
+  <si>
+    <t>? Nd</t>
+  </si>
+  <si>
+    <t>---ok</t>
+  </si>
+  <si>
+    <t>no: method getPaymentAppliedAmount should be moved at the end or before the first getPaymentNotApplied</t>
   </si>
 </sst>
 </file>
@@ -406,11 +439,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -424,6 +454,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -742,612 +775,642 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView topLeftCell="A7" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="127.28515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="127.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>95</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>97</v>
       </c>
     </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+      <c r="A97" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
+      <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+      <c r="A100" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+      <c r="A101" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+      <c r="A102" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
+      <c r="A103" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
+      <c r="A104" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="4" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
+      <c r="A140" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
+      <c r="A144" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
+      <c r="A147" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
+      <c r="A150" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="4" t="s">
+      <c r="A153" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
+      <c r="A154" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
+      <c r="A158" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
+      <c r="A161" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
+      <c r="A164" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
+      <c r="A167" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
+      <c r="A168" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
+      <c r="A171" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
+      <c r="A174" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
+      <c r="A177" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
+      <c r="A180" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="5" t="s">
+      <c r="A183" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="5" t="s">
+      <c r="A186" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="5" t="s">
+      <c r="A189" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="4" t="s">
+      <c r="A192" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="5" t="s">
+      <c r="A193" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
+      <c r="A196" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="4" t="s">
+      <c r="A199" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="5" t="s">
+      <c r="A200" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="5" t="s">
+      <c r="A203" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="5" t="s">
+      <c r="A206" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="4" t="s">
+      <c r="A209" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="5" t="s">
+      <c r="A210" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="5" t="s">
+      <c r="A213" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="5" t="s">
+      <c r="A216" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="5" t="s">
+      <c r="A219" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1361,477 +1424,582 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A219"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="228" customWidth="1"/>
+    <col min="1" max="1" width="228" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="5" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="2" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="2" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
+      <c r="A167" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
+      <c r="A177" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="3" t="s">
+      <c r="A180" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="3" t="s">
+      <c r="A189" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
+      <c r="A193" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="3" t="s">
+      <c r="A196" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
+      <c r="A199" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
+      <c r="A200" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="3" t="s">
+      <c r="A203" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="3" t="s">
+      <c r="A206" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
+      <c r="A209" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished code inspection - review needed for questions
</commit_message>
<xml_diff>
--- a/5_CodeInspection/Code_checks_Erica_v1.xlsx
+++ b/5_CodeInspection/Code_checks_Erica_v1.xlsx
@@ -16,6 +16,7 @@
     <sheet name="PaymentWorker" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="126">
   <si>
     <t>2.1 Naming Conventions</t>
   </si>
@@ -360,9 +361,6 @@
     <t xml:space="preserve">getPaymentMethodAndRelated: lines 103, 107, </t>
   </si>
   <si>
-    <t>ok blanks, comments are missing</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -379,6 +377,33 @@
   </si>
   <si>
     <t>no: method getPaymentAppliedAmount should be moved at the end or before the first getPaymentNotApplied</t>
+  </si>
+  <si>
+    <t>getPaymentMethodAndRelated: lines 106, 111, 120, 121, 122, 123, 124, 156 should be moved on the top of the method.</t>
+  </si>
+  <si>
+    <t>getPaymentMethodAndRelated: lines 143-152 and 158-165 performs the same checks. Group them.</t>
+  </si>
+  <si>
+    <t>---?</t>
+  </si>
+  <si>
+    <t>ok blanks, comments are missing. New lines could be added in method getPaymentApplied.</t>
+  </si>
+  <si>
+    <t>in getPaymentApplied is not checked that actualCurrencyAmount is different from zero</t>
+  </si>
+  <si>
+    <t>ok?</t>
+  </si>
+  <si>
+    <t>ok ---?</t>
+  </si>
+  <si>
+    <t>---? Getattribute?</t>
+  </si>
+  <si>
+    <t>just log. Is appropriate??? ---?</t>
   </si>
 </sst>
 </file>
@@ -1422,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A219"/>
+  <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1565,7 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -1550,7 +1575,7 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -1560,7 +1585,7 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -1665,7 +1690,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
@@ -1680,7 +1705,7 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
@@ -1780,7 +1805,7 @@
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
@@ -1790,7 +1815,7 @@
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
@@ -1803,31 +1828,61 @@
         <v>46</v>
       </c>
     </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>48</v>
       </c>
     </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>52</v>
@@ -1858,16 +1913,31 @@
         <v>57</v>
       </c>
     </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>58</v>
       </c>
     </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>60</v>
@@ -1878,6 +1948,11 @@
         <v>61</v>
       </c>
     </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>62</v>
@@ -1888,16 +1963,31 @@
         <v>63</v>
       </c>
     </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>64</v>
       </c>
     </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>66</v>
@@ -1908,41 +1998,86 @@
         <v>92</v>
       </c>
     </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>69</v>
       </c>
     </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>73</v>
       </c>
     </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>74</v>
@@ -1953,11 +2088,21 @@
         <v>75</v>
       </c>
     </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>76</v>
       </c>
     </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>77</v>
@@ -1968,16 +2113,31 @@
         <v>78</v>
       </c>
     </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>81</v>
@@ -1988,22 +2148,43 @@
         <v>82</v>
       </c>
     </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>83</v>
       </c>
     </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>85</v>
       </c>
     </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added erica's check list
</commit_message>
<xml_diff>
--- a/5_CodeInspection/Code_checks_Erica_v1.xlsx
+++ b/5_CodeInspection/Code_checks_Erica_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BillingAccountWorker" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +450,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -463,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -481,6 +487,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A221" sqref="A221"/>
+    <sheetView topLeftCell="A198" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A227" sqref="A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1071,7 @@
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1174,7 +1186,7 @@
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="7" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1568,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,16 +2054,25 @@
         <v>53</v>
       </c>
     </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="7"/>
+    </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>54</v>
       </c>
     </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="7"/>
+    </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="7"/>
+    </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>56</v>
@@ -2223,7 +2244,7 @@
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="6" t="s">
+      <c r="A190" s="8" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2248,7 +2269,7 @@
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="4" t="s">
+      <c r="A197" s="7" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2299,7 +2320,7 @@
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
@@ -2309,7 +2330,7 @@
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
@@ -2319,7 +2340,7 @@
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
@@ -2329,7 +2350,7 @@
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>